<commit_message>
type: feat Save the excel report
</commit_message>
<xml_diff>
--- a/POS Code/Experiments/attachments/ICSE/summary.xlsx
+++ b/POS Code/Experiments/attachments/ICSE/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuh/Documents/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zefuhu/Documents/workspace/papers/PhD_research/NLP/probing/datasets_creation/cubert/interpretability-of-source-code-transformers/POS Code/Experiments/attachments/ICSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8534AAC5-DBDC-C647-A290-B6FA49F32F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF50A8-2A46-A34A-8ECB-5379EDDBF9B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1000" windowWidth="27640" windowHeight="15760"/>
+    <workbookView xWindow="12720" yWindow="4960" windowWidth="25940" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,32 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>Selection</t>
   </si>
   <si>
-    <t>Token tagging</t>
-  </si>
-  <si>
     <t>Code Search</t>
   </si>
   <si>
-    <t>DefDect</t>
-  </si>
-  <si>
-    <t>CloneDetction</t>
-  </si>
-  <si>
-    <t>CodeBERT</t>
-  </si>
-  <si>
-    <t>GraphCodeBERT</t>
-  </si>
-  <si>
-    <t>UniXCoder</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
@@ -89,10 +67,6 @@
   </si>
   <si>
     <t>1-1</t>
-  </si>
-  <si>
-    <t>CodeGPTPy
-Adapted</t>
   </si>
   <si>
     <t>LS+
@@ -112,17 +86,44 @@
     <t>0-12</t>
   </si>
   <si>
-    <t>0-2</t>
-  </si>
-  <si>
-    <t>All</t>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>GCB</t>
+  </si>
+  <si>
+    <t>CGPA</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>Diff.</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Defect Detection</t>
+  </si>
+  <si>
+    <t>Clone Detection</t>
+  </si>
+  <si>
+    <t>Token Tagging(Python)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,6 +257,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -599,37 +614,44 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -986,11 +1008,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,75 +1030,76 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="N1" s="3"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>9984</v>
@@ -1084,97 +1107,97 @@
       <c r="D3" s="2">
         <v>9984</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>9984</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>9984</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>9984</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>9984</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="4">
         <v>9984</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="4">
         <v>9984</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="4">
         <v>9984</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <v>9984</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="4">
         <v>9984</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="4">
         <v>9984</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="4">
         <v>9984</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5">
         <v>0.91459999999999997</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>0.89290000000000003</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>0.83579999999999999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>0.96009999999999995</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.47520000000000001</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.50329999999999997</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.48680000000000001</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="G4" s="5">
+        <v>0.54139999999999999</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.4652</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.50990000000000002</v>
+      </c>
+      <c r="J4" s="5">
         <v>0.64019999999999999</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="5">
         <v>0.63870000000000005</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="5">
         <v>0.66800000000000004</v>
       </c>
       <c r="M4" s="2">
-        <v>0.25</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="N4" s="2">
-        <v>0.56999999999999995</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="O4" s="2">
-        <v>0.21</v>
+        <v>0.82799999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
         <v>0.5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
         <v>0.7</v>
@@ -1183,10 +1206,10 @@
         <v>0.4</v>
       </c>
       <c r="G5" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>0.9</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.5</v>
       </c>
       <c r="I5" s="2">
         <v>0.8</v>
@@ -1201,19 +1224,19 @@
         <v>0.2</v>
       </c>
       <c r="M5" s="2">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="N5" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="O5" s="2">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>3229</v>
@@ -1228,13 +1251,13 @@
         <v>3406</v>
       </c>
       <c r="G6" s="2">
-        <v>1066</v>
+        <v>768</v>
       </c>
       <c r="H6" s="2">
-        <v>8777</v>
+        <v>1454</v>
       </c>
       <c r="I6" s="2">
-        <v>1092</v>
+        <v>768</v>
       </c>
       <c r="J6" s="2">
         <v>1742</v>
@@ -1246,399 +1269,520 @@
         <v>8890</v>
       </c>
       <c r="M6" s="2">
-        <v>771</v>
+        <v>2264</v>
       </c>
       <c r="N6" s="2">
-        <v>6688</v>
+        <v>6124</v>
       </c>
       <c r="O6" s="2">
-        <v>771</v>
+        <v>901</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
         <v>0.94930000000000003</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="5">
         <v>0.98209999999999997</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>0.98799999999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
         <v>0.99029999999999996</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.51659999999999995</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.51819999999999999</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.50170000000000003</v>
-      </c>
-      <c r="J7" s="3">
+      <c r="G7" s="5">
+        <v>0.55459999999999998</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.53480000000000005</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.5232</v>
+      </c>
+      <c r="J7" s="5">
         <v>0.6552</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="5">
         <v>0.64349999999999996</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="5">
         <v>0.67020000000000002</v>
       </c>
-      <c r="M7" s="7">
-        <v>0.67</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="O7" s="11">
-        <v>0.67</v>
+      <c r="M7" s="8">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.80500000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5">
+        <f>C7-C4</f>
+        <v>3.4700000000000064E-2</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ref="D8:O8" si="0">D7-D4</f>
+        <v>8.9199999999999946E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1522</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0200000000000005E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.319999999999999E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>6.9600000000000051E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3299999999999979E-2</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>4.7999999999999154E-3</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999797E-3</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999904E-2</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="0"/>
+        <v>-2.2999999999999909E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5">
         <v>0.67659999999999998</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E9" s="7">
         <v>0.9355</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="5">
         <v>0.65890000000000004</v>
       </c>
-      <c r="G8" s="3">
-        <f>1-G6/9984</f>
-        <v>0.89322916666666663</v>
-      </c>
-      <c r="H8" s="3">
-        <f>1-H6/9984</f>
-        <v>0.12089342948717952</v>
-      </c>
-      <c r="I8" s="3">
-        <f>1-I6/I3</f>
-        <v>0.890625</v>
-      </c>
-      <c r="J8" s="3">
+      <c r="G9" s="5">
+        <f>1-G6/G3</f>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" ref="H9:I9" si="1">1-H6/H3</f>
+        <v>0.85436698717948723</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="J9" s="5">
         <f>1-J6/J3</f>
         <v>0.82552083333333337</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K9" s="5">
         <v>0.74409999999999998</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L9" s="5">
         <v>0.1096</v>
       </c>
-      <c r="M8" s="3">
-        <f>1-M6/9984</f>
-        <v>0.92277644230769229</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0.3301</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="M9" s="5">
+        <f>1-M6/M3</f>
+        <v>0.77323717948717952</v>
+      </c>
+      <c r="N9" s="5">
+        <f>1-N6/N3</f>
+        <v>0.38661858974358976</v>
+      </c>
+      <c r="O9" s="5">
         <f>1-O6/O3</f>
-        <v>0.92277644230769229</v>
+        <v>0.90975560897435903</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="N10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2">
-        <v>49</v>
-      </c>
-      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="2">
-        <v>199</v>
+        <v>0.3</v>
       </c>
       <c r="G12" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="2">
+      <c r="K12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="2">
+      <c r="O12" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="J12" s="2">
-        <v>99</v>
-      </c>
-      <c r="K12" s="2">
-        <v>399</v>
-      </c>
-      <c r="L12" s="2">
-        <v>29</v>
-      </c>
-      <c r="M12" s="2">
-        <v>9</v>
-      </c>
-      <c r="N12" s="2">
-        <v>29</v>
-      </c>
-      <c r="O12" s="2">
-        <v>1996</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0.94179999999999997</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.89590000000000003</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.87</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.99029999999999996</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0.48180000000000001</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0.48180000000000001</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0.48180000000000001</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0.65149999999999997</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.63649999999999995</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.65559999999999996</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0.67</v>
-      </c>
-      <c r="N13" s="11">
-        <v>0.67</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="2">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2">
+        <v>49</v>
+      </c>
+      <c r="E13" s="2">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2">
+        <v>199</v>
+      </c>
+      <c r="G13" s="12">
+        <v>399</v>
+      </c>
+      <c r="H13" s="2">
+        <v>399</v>
+      </c>
+      <c r="I13" s="2">
+        <v>499</v>
+      </c>
+      <c r="J13" s="2">
+        <v>99</v>
+      </c>
+      <c r="K13" s="2">
+        <v>399</v>
+      </c>
+      <c r="L13" s="2">
+        <v>29</v>
+      </c>
+      <c r="M13" s="2">
+        <v>19</v>
+      </c>
+      <c r="N13" s="2">
+        <v>19</v>
       </c>
       <c r="O13" s="2">
-        <v>0.67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.99509999999999998</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.99909999999999999</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0.98009999999999997</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0.99909999999999999</v>
-      </c>
-      <c r="H14" s="9">
-        <f>1-H12/9984</f>
-        <v>0.99909855769230771</v>
-      </c>
-      <c r="I14" s="9">
-        <v>0.99909999999999999</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0.99009999999999998</v>
-      </c>
-      <c r="K14" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="M14" s="9">
-        <f>1-M12/9984</f>
-        <v>0.99909855769230771</v>
-      </c>
-      <c r="N14" s="9">
-        <v>0.99709999999999999</v>
-      </c>
-      <c r="O14" s="3">
-        <v>0.80010000000000003</v>
+        <v>5</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.94179999999999997</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.89590000000000003</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.53310000000000002</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.5232</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.63649999999999995</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.65559999999999996</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="N14" s="14">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0.83099999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11">
+        <f>C14-C4</f>
+        <v>2.7200000000000002E-2</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" ref="D15:O15" si="2">D14-D4</f>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="E15" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4200000000000008E-2</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="2"/>
+        <v>3.0200000000000005E-2</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="2"/>
+        <v>-3.2999999999999696E-3</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="2"/>
+        <v>6.7900000000000016E-2</v>
+      </c>
+      <c r="I15" s="11">
+        <f t="shared" si="2"/>
+        <v>1.3299999999999979E-2</v>
+      </c>
+      <c r="J15" s="11">
+        <f t="shared" si="2"/>
+        <v>1.1299999999999977E-2</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="2"/>
+        <v>-2.2000000000000908E-3</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="2"/>
+        <v>-1.2400000000000078E-2</v>
+      </c>
+      <c r="M15" s="13">
+        <f t="shared" si="2"/>
+        <v>-7.0000000000000062E-3</v>
+      </c>
+      <c r="N15" s="13">
+        <f t="shared" si="2"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="2"/>
+        <v>3.0000000000000027E-3</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.98009999999999997</v>
+      </c>
+      <c r="G16" s="7">
+        <f>1-G13/G3</f>
+        <v>0.96003605769230771</v>
+      </c>
+      <c r="H16" s="7">
+        <f>1-H13/H3</f>
+        <v>0.96003605769230771</v>
+      </c>
+      <c r="I16" s="7">
+        <f>1-I13/I3</f>
+        <v>0.95002003205128205</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.99009999999999998</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="M16" s="7">
+        <f>1-M13/M3</f>
+        <v>0.99809695512820518</v>
+      </c>
+      <c r="N16" s="7">
+        <f>1-N13/N3</f>
+        <v>0.99809695512820518</v>
+      </c>
+      <c r="O16" s="7">
+        <f>1-O13/O3</f>
+        <v>0.99008413461538458</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>